<commit_message>
refactor holiday added families file properties to be regular families file properties (added driver prop)
</commit_message>
<xml_diff>
--- a/backend/system_files/holiday_template.xlsx
+++ b/backend/system_files/holiday_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\shalom\gmah\backend\system_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA342B90-3EF6-4976-96BC-0DA48A87D779}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD7BC86B-DFC6-4F79-8CC2-72A34C9D99CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>שם מלא</t>
   </si>
@@ -47,6 +47,9 @@
   </si>
   <si>
     <t>הערות</t>
+  </si>
+  <si>
+    <t>נהג</t>
   </si>
 </sst>
 </file>
@@ -163,7 +166,15 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="שורת נתמך" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="3">
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <border outline="0">
         <top style="thin">
@@ -207,12 +218,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="נתמכים" displayName="נתמכים" ref="A1:I2" insertRow="1" totalsRowShown="0" headerRowDxfId="1" tableBorderDxfId="0" dataCellStyle="שורת נתמך">
-  <autoFilter ref="A1:I2" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I2">
-    <sortCondition ref="H1:H2"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="נתמכים" displayName="נתמכים" ref="A1:J2" insertRow="1" totalsRowShown="0" headerRowDxfId="2" tableBorderDxfId="1" dataCellStyle="שורת נתמך">
+  <autoFilter ref="A1:J2" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J2">
+    <sortCondition ref="I1:I2"/>
   </sortState>
-  <tableColumns count="9">
+  <tableColumns count="10">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="שם מלא" dataCellStyle="שורת נתמך"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="רחוב" dataCellStyle="שורת נתמך"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="בניין" dataCellStyle="שורת נתמך"/>
@@ -220,6 +231,7 @@
     <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="קומה" dataCellStyle="שורת נתמך"/>
     <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="מס' בית" dataCellStyle="שורת נתמך"/>
     <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="מס' פלאפון" dataCellStyle="שורת נתמך"/>
+    <tableColumn id="10" xr3:uid="{4323218E-C5B3-40A0-AD9A-8BDCA8210423}" name="נהג" dataDxfId="0" dataCellStyle="שורת נתמך"/>
     <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="ממליץ" dataCellStyle="שורת נתמך"/>
     <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="הערות" dataCellStyle="שורת נתמך"/>
   </tableColumns>
@@ -524,10 +536,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.80859375" defaultRowHeight="14.4" x14ac:dyDescent="0.45"/>
@@ -537,13 +549,14 @@
     <col min="3" max="5" width="8.80859375" style="4" customWidth="1"/>
     <col min="6" max="6" width="12.09375" style="4" customWidth="1"/>
     <col min="7" max="7" width="12.85546875" style="4" customWidth="1"/>
-    <col min="8" max="8" width="15.5234375" style="4" customWidth="1"/>
-    <col min="9" max="9" width="24.5234375" style="4" customWidth="1"/>
-    <col min="10" max="12" width="8.80859375" style="4" customWidth="1"/>
-    <col min="13" max="16384" width="8.80859375" style="4"/>
+    <col min="8" max="8" width="13.76171875" style="4" customWidth="1"/>
+    <col min="9" max="9" width="15.5234375" style="4" customWidth="1"/>
+    <col min="10" max="10" width="24.5234375" style="4" customWidth="1"/>
+    <col min="11" max="13" width="8.80859375" style="4" customWidth="1"/>
+    <col min="14" max="16384" width="8.80859375" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="14.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:10" ht="14.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -565,14 +578,17 @@
       <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="14.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:10" ht="14.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A2" s="5"/>
       <c r="B2" s="5"/>
       <c r="C2" s="5"/>
@@ -582,6 +598,7 @@
       <c r="G2" s="5"/>
       <c r="H2" s="5"/>
       <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>